<commit_message>
Modified code to get urls from excel
</commit_message>
<xml_diff>
--- a/resources/datarepo/htmllinks.xlsx
+++ b/resources/datarepo/htmllinks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\NextGen Cloudlabs\Presentation\Free Labs Session\DevOps-CICD-Automation-Demo\resources\datarepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41FD483-A248-41D8-BC50-C85919B9AA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE8E26A-D1E2-4DF2-A9ED-179D1C7FD560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>http://172.31.21.30:8082/webapp/</t>
   </si>
@@ -33,10 +33,13 @@
     <t>test-link1</t>
   </si>
   <si>
-    <t>test-link2</t>
+    <t>http://172.31.21.30:8083</t>
   </si>
   <si>
-    <t>http://172.31.21.30:8083</t>
+    <t>http://172.31.25.94:8082/webapp/</t>
+  </si>
+  <si>
+    <t>http://172.31.25.94:8083</t>
   </si>
 </sst>
 </file>
@@ -371,72 +374,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B105"/>
+  <dimension ref="A1:A105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.42578125" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -710,7 +712,9 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{E9D2779F-6A56-429A-ADEF-22EBC65A0B99}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{41D39225-42CE-45B8-AA8F-34E2813F9C75}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{E13879C1-E984-4B1B-AF36-0556F5B3FB7A}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{ADF863C2-CD5C-4D53-8C03-0481A04AA62F}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{F677DD57-D2EC-4DCE-88A0-5A9A9B26CA91}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>